<commit_message>
moving to new windows install
</commit_message>
<xml_diff>
--- a/assignment2docs/mc_vs_pi.xlsx
+++ b/assignment2docs/mc_vs_pi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b01759976628a285/School/Search_Engines/assignment2docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick Anderson\OneDrive\School\Search_Engines\assignment2docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -284,7 +284,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$9:$A$13</c:f>
+              <c:f>Sheet1!$A$14:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -308,24 +308,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$B$13</c:f>
+              <c:f>Sheet1!$B$14:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7.2841918958479804E-7</c:v>
+                  <c:v>1.4510244008709099E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.7799977523737404E-7</c:v>
+                  <c:v>7.0686529086884303E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6780930317487401E-7</c:v>
+                  <c:v>1.5974736883292899E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2918945093584899E-8</c:v>
+                  <c:v>2.3960736152945901E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8605569800906203E-9</c:v>
+                  <c:v>3.8580355346083702E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -366,7 +366,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$20</c:f>
+              <c:f>Sheet1!$A$23:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -390,24 +390,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$B$20</c:f>
+              <c:f>Sheet1!$B$23:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.8380796289791E-7</c:v>
+                  <c:v>1.7932944029196901E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3675456029753599E-7</c:v>
+                  <c:v>3.7246370449146702E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9183071390736901E-8</c:v>
+                  <c:v>1.0453911621326E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1301042511442001E-8</c:v>
+                  <c:v>1.27952673553787E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.50885690802169E-9</c:v>
+                  <c:v>1.70838200365653E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -448,7 +448,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$23:$A$27</c:f>
+              <c:f>Sheet1!$A$33:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -472,24 +472,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$23:$B$27</c:f>
+              <c:f>Sheet1!$B$33:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.2226509928910699E-7</c:v>
+                  <c:v>6.7026041219985505E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2018927582180697E-8</c:v>
+                  <c:v>5.4946485086662899E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1548136916757099E-8</c:v>
+                  <c:v>9.9410512173473498E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6582931970523899E-9</c:v>
+                  <c:v>1.97341778817197E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.6371932109278102E-10</c:v>
+                  <c:v>4.8655405956019296E-10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -530,7 +530,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$30:$A$34</c:f>
+              <c:f>Sheet1!$A$44:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -554,24 +554,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$30:$B$34</c:f>
+              <c:f>Sheet1!$B$44:$B$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.3131755228371001E-7</c:v>
+                  <c:v>6.3325189237862194E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.46869455247919E-7</c:v>
+                  <c:v>1.16774127528446E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1461888292308501E-8</c:v>
+                  <c:v>4.4652915683968E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0066208912654796E-9</c:v>
+                  <c:v>3.8425043965408002E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.9031282642286391E-10</c:v>
+                  <c:v>1.1005629710667E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -612,7 +612,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$37:$A$41</c:f>
+              <c:f>Sheet1!$A$54:$A$58</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -636,24 +636,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$37:$B$41</c:f>
+              <c:f>Sheet1!$B$54:$B$58</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.2329631936035599E-7</c:v>
+                  <c:v>5.6771458938979796E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1163338770654499E-7</c:v>
+                  <c:v>2.1569138208979601E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.1843696559632905E-8</c:v>
+                  <c:v>4.43760945555107E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.77673000217923E-9</c:v>
+                  <c:v>4.7120170133968798E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.00435672696243E-9</c:v>
+                  <c:v>8.1723315720573001E-10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -704,7 +704,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$9:$A$13</c:f>
+              <c:f>Sheet1!$A$14:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -728,24 +728,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$B$13</c:f>
+              <c:f>Sheet1!$B$14:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7.2841918958479804E-7</c:v>
+                  <c:v>1.4510244008709099E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.7799977523737404E-7</c:v>
+                  <c:v>7.0686529086884303E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6780930317487401E-7</c:v>
+                  <c:v>1.5974736883292899E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2918945093584899E-8</c:v>
+                  <c:v>2.3960736152945901E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8605569800906203E-9</c:v>
+                  <c:v>3.8580355346083702E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -796,7 +796,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$20</c:f>
+              <c:f>Sheet1!$A$23:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -820,24 +820,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$B$20</c:f>
+              <c:f>Sheet1!$B$23:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.8380796289791E-7</c:v>
+                  <c:v>1.7932944029196901E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3675456029753599E-7</c:v>
+                  <c:v>3.7246370449146702E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9183071390736901E-8</c:v>
+                  <c:v>1.0453911621326E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1301042511442001E-8</c:v>
+                  <c:v>1.27952673553787E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.50885690802169E-9</c:v>
+                  <c:v>1.70838200365653E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -888,7 +888,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$23:$A$27</c:f>
+              <c:f>Sheet1!$A$33:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -912,24 +912,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$23:$B$27</c:f>
+              <c:f>Sheet1!$B$33:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.2226509928910699E-7</c:v>
+                  <c:v>6.7026041219985505E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2018927582180697E-8</c:v>
+                  <c:v>5.4946485086662899E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1548136916757099E-8</c:v>
+                  <c:v>9.9410512173473498E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6582931970523899E-9</c:v>
+                  <c:v>1.97341778817197E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.6371932109278102E-10</c:v>
+                  <c:v>4.8655405956019296E-10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -980,7 +980,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$30:$A$34</c:f>
+              <c:f>Sheet1!$A$44:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1004,24 +1004,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$30:$B$34</c:f>
+              <c:f>Sheet1!$B$44:$B$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.3131755228371001E-7</c:v>
+                  <c:v>6.3325189237862194E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.46869455247919E-7</c:v>
+                  <c:v>1.16774127528446E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1461888292308501E-8</c:v>
+                  <c:v>4.4652915683968E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0066208912654796E-9</c:v>
+                  <c:v>3.8425043965408002E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.9031282642286391E-10</c:v>
+                  <c:v>1.1005629710667E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1072,7 +1072,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$37:$A$41</c:f>
+              <c:f>Sheet1!$A$54:$A$58</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1096,24 +1096,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$37:$B$41</c:f>
+              <c:f>Sheet1!$B$54:$B$58</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.2329631936035599E-7</c:v>
+                  <c:v>5.6771458938979796E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1163338770654499E-7</c:v>
+                  <c:v>2.1569138208979601E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.1843696559632905E-8</c:v>
+                  <c:v>4.43760945555107E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.77673000217923E-9</c:v>
+                  <c:v>4.7120170133968798E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.00435672696243E-9</c:v>
+                  <c:v>8.1723315720573001E-10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1128,11 +1128,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="281997792"/>
-        <c:axId val="281995048"/>
+        <c:axId val="323970920"/>
+        <c:axId val="323973272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="281997792"/>
+        <c:axId val="323970920"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1239,12 +1239,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="281995048"/>
+        <c:crossAx val="323973272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="281995048"/>
+        <c:axId val="323973272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1372,7 +1372,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="281997792"/>
+        <c:crossAx val="323970920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1583,7 +1583,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$9:$A$13</c:f>
+              <c:f>Sheet1!$A$14:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1607,24 +1607,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$B$13</c:f>
+              <c:f>Sheet1!$B$14:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7.2841918958479804E-7</c:v>
+                  <c:v>1.4510244008709099E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.7799977523737404E-7</c:v>
+                  <c:v>7.0686529086884303E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6780930317487401E-7</c:v>
+                  <c:v>1.5974736883292899E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2918945093584899E-8</c:v>
+                  <c:v>2.3960736152945901E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8605569800906203E-9</c:v>
+                  <c:v>3.8580355346083702E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1665,7 +1665,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$20</c:f>
+              <c:f>Sheet1!$A$23:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1689,24 +1689,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$B$20</c:f>
+              <c:f>Sheet1!$B$23:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.8380796289791E-7</c:v>
+                  <c:v>1.7932944029196901E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3675456029753599E-7</c:v>
+                  <c:v>3.7246370449146702E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9183071390736901E-8</c:v>
+                  <c:v>1.0453911621326E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1301042511442001E-8</c:v>
+                  <c:v>1.27952673553787E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.50885690802169E-9</c:v>
+                  <c:v>1.70838200365653E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1747,7 +1747,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$23:$A$27</c:f>
+              <c:f>Sheet1!$A$33:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1771,24 +1771,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$23:$B$27</c:f>
+              <c:f>Sheet1!$B$33:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.2226509928910699E-7</c:v>
+                  <c:v>6.7026041219985505E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2018927582180697E-8</c:v>
+                  <c:v>5.4946485086662899E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1548136916757099E-8</c:v>
+                  <c:v>9.9410512173473498E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6582931970523899E-9</c:v>
+                  <c:v>1.97341778817197E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.6371932109278102E-10</c:v>
+                  <c:v>4.8655405956019296E-10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1829,7 +1829,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$30:$A$34</c:f>
+              <c:f>Sheet1!$A$44:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1853,24 +1853,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$30:$B$34</c:f>
+              <c:f>Sheet1!$B$44:$B$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.3131755228371001E-7</c:v>
+                  <c:v>6.3325189237862194E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.46869455247919E-7</c:v>
+                  <c:v>1.16774127528446E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1461888292308501E-8</c:v>
+                  <c:v>4.4652915683968E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0066208912654796E-9</c:v>
+                  <c:v>3.8425043965408002E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.9031282642286391E-10</c:v>
+                  <c:v>1.1005629710667E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1911,7 +1911,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$37:$A$41</c:f>
+              <c:f>Sheet1!$A$54:$A$58</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1935,24 +1935,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$37:$B$41</c:f>
+              <c:f>Sheet1!$B$54:$B$58</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.2329631936035599E-7</c:v>
+                  <c:v>5.6771458938979796E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1163338770654499E-7</c:v>
+                  <c:v>2.1569138208979601E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.1843696559632905E-8</c:v>
+                  <c:v>4.43760945555107E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.77673000217923E-9</c:v>
+                  <c:v>4.7120170133968798E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.00435672696243E-9</c:v>
+                  <c:v>8.1723315720573001E-10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2003,7 +2003,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$9:$A$13</c:f>
+              <c:f>Sheet1!$A$14:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2027,24 +2027,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$B$13</c:f>
+              <c:f>Sheet1!$B$14:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7.2841918958479804E-7</c:v>
+                  <c:v>1.4510244008709099E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.7799977523737404E-7</c:v>
+                  <c:v>7.0686529086884303E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6780930317487401E-7</c:v>
+                  <c:v>1.5974736883292899E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2918945093584899E-8</c:v>
+                  <c:v>2.3960736152945901E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8605569800906203E-9</c:v>
+                  <c:v>3.8580355346083702E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2095,7 +2095,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$20</c:f>
+              <c:f>Sheet1!$A$23:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2119,24 +2119,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$B$20</c:f>
+              <c:f>Sheet1!$B$23:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.8380796289791E-7</c:v>
+                  <c:v>1.7932944029196901E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3675456029753599E-7</c:v>
+                  <c:v>3.7246370449146702E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9183071390736901E-8</c:v>
+                  <c:v>1.0453911621326E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1301042511442001E-8</c:v>
+                  <c:v>1.27952673553787E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.50885690802169E-9</c:v>
+                  <c:v>1.70838200365653E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2187,7 +2187,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$23:$A$27</c:f>
+              <c:f>Sheet1!$A$33:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2211,24 +2211,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$23:$B$27</c:f>
+              <c:f>Sheet1!$B$33:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.2226509928910699E-7</c:v>
+                  <c:v>6.7026041219985505E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2018927582180697E-8</c:v>
+                  <c:v>5.4946485086662899E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1548136916757099E-8</c:v>
+                  <c:v>9.9410512173473498E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6582931970523899E-9</c:v>
+                  <c:v>1.97341778817197E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.6371932109278102E-10</c:v>
+                  <c:v>4.8655405956019296E-10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2279,7 +2279,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$30:$A$34</c:f>
+              <c:f>Sheet1!$A$44:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2303,24 +2303,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$30:$B$34</c:f>
+              <c:f>Sheet1!$B$44:$B$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.3131755228371001E-7</c:v>
+                  <c:v>6.3325189237862194E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.46869455247919E-7</c:v>
+                  <c:v>1.16774127528446E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1461888292308501E-8</c:v>
+                  <c:v>4.4652915683968E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0066208912654796E-9</c:v>
+                  <c:v>3.8425043965408002E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.9031282642286391E-10</c:v>
+                  <c:v>1.1005629710667E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2371,7 +2371,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$37:$A$41</c:f>
+              <c:f>Sheet1!$A$54:$A$58</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2395,24 +2395,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$37:$B$41</c:f>
+              <c:f>Sheet1!$B$54:$B$58</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.2329631936035599E-7</c:v>
+                  <c:v>5.6771458938979796E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1163338770654499E-7</c:v>
+                  <c:v>2.1569138208979601E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.1843696559632905E-8</c:v>
+                  <c:v>4.43760945555107E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.77673000217923E-9</c:v>
+                  <c:v>4.7120170133968798E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.00435672696243E-9</c:v>
+                  <c:v>8.1723315720573001E-10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2427,11 +2427,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="455214584"/>
-        <c:axId val="455214976"/>
+        <c:axId val="323972096"/>
+        <c:axId val="323967784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="455214584"/>
+        <c:axId val="323972096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2530,12 +2530,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455214976"/>
+        <c:crossAx val="323967784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="455214976"/>
+        <c:axId val="323967784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2663,7 +2663,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455214584"/>
+        <c:crossAx val="323972096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2837,7 +2837,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15296453871253279"/>
+          <c:y val="1.1235247446036828E-2"/>
+          <c:w val="0.75138888528360459"/>
+          <c:h val="0.80833494132158268"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -2885,7 +2895,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$9:$A$13</c:f>
+              <c:f>Sheet1!$A$14:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2909,24 +2919,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$9:$C$13</c:f>
+              <c:f>Sheet1!$C$14:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.8084443910738601E-4</c:v>
+                  <c:v>2.1857214590375499E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8084443910738601E-4</c:v>
+                  <c:v>2.1857214590375499E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8084443910738601E-4</c:v>
+                  <c:v>2.1857214590375499E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7876878651046302E-4</c:v>
+                  <c:v>3.0640327873730502E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.77846248916882E-4</c:v>
+                  <c:v>3.1520405020451002E-10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2977,7 +2987,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$20</c:f>
+              <c:f>Sheet1!$A$23:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3001,24 +3011,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$20</c:f>
+              <c:f>Sheet1!$C$23:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.3614813035795307E-5</c:v>
+                  <c:v>7.2857381967918304E-9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.3614813035795307E-5</c:v>
+                  <c:v>7.2857381967918304E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.3614813035795307E-5</c:v>
+                  <c:v>7.2857381967918304E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2913205979498306E-5</c:v>
+                  <c:v>1.00899149306323E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.2618474537597097E-5</c:v>
+                  <c:v>1.04452939783475E-10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3069,7 +3079,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$23:$A$27</c:f>
+              <c:f>Sheet1!$A$33:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3093,24 +3103,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$23:$C$27</c:f>
+              <c:f>Sheet1!$C$33:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.3275327478062006E-5</c:v>
+                  <c:v>3.6133495493571098E-9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.3272685862591802E-5</c:v>
+                  <c:v>3.58601761314407E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.2933827343348602E-5</c:v>
+                  <c:v>9.8266068191216605E-10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2617904601325404E-5</c:v>
+                  <c:v>1.02034131630548E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.2518006423951497E-5</c:v>
+                  <c:v>1.15981075032377E-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3161,7 +3171,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$30:$A$34</c:f>
+              <c:f>Sheet1!$A$44:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3185,24 +3195,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$C$34</c:f>
+              <c:f>Sheet1!$C$44:$C$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.2465522705215594E-5</c:v>
+                  <c:v>7.2552432449926497E-14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.24643500220788E-5</c:v>
+                  <c:v>8.5630497752193801E-15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.2466296799958707E-5</c:v>
+                  <c:v>1.9967450179935801E-18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2468291488930903E-5</c:v>
+                  <c:v>2.23770026259195E-15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.2467334264881597E-5</c:v>
+                  <c:v>1.25480053373134E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3253,7 +3263,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$37:$A$41</c:f>
+              <c:f>Sheet1!$A$54:$A$58</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3277,24 +3287,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$37:$C$41</c:f>
+              <c:f>Sheet1!$C$54:$C$58</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.3614813035795307E-5</c:v>
+                  <c:v>7.2857381967918304E-9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.3614813035795307E-5</c:v>
+                  <c:v>7.2857381967918304E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.3455513367966293E-5</c:v>
+                  <c:v>4.1005294095570102E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2810567711688194E-5</c:v>
+                  <c:v>5.2462033741270401E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.2566615498012401E-5</c:v>
+                  <c:v>5.5698133673293799E-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3309,11 +3319,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="576079632"/>
-        <c:axId val="576080024"/>
+        <c:axId val="323966216"/>
+        <c:axId val="323972880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="576079632"/>
+        <c:axId val="323966216"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3414,12 +3424,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="576080024"/>
+        <c:crossAx val="323972880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="576080024"/>
+        <c:axId val="323972880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3551,7 +3561,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="576079632"/>
+        <c:crossAx val="323966216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3764,7 +3774,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$9:$A$13</c:f>
+              <c:f>Sheet1!$A$14:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3788,24 +3798,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$9:$C$13</c:f>
+              <c:f>Sheet1!$C$14:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.8084443910738601E-4</c:v>
+                  <c:v>2.1857214590375499E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8084443910738601E-4</c:v>
+                  <c:v>2.1857214590375499E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8084443910738601E-4</c:v>
+                  <c:v>2.1857214590375499E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7876878651046302E-4</c:v>
+                  <c:v>3.0640327873730502E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.77846248916882E-4</c:v>
+                  <c:v>3.1520405020451002E-10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3856,7 +3866,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$20</c:f>
+              <c:f>Sheet1!$A$23:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3880,24 +3890,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$20</c:f>
+              <c:f>Sheet1!$C$23:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.3614813035795307E-5</c:v>
+                  <c:v>7.2857381967918304E-9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.3614813035795307E-5</c:v>
+                  <c:v>7.2857381967918304E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.3614813035795307E-5</c:v>
+                  <c:v>7.2857381967918304E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2913205979498306E-5</c:v>
+                  <c:v>1.00899149306323E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.2618474537597097E-5</c:v>
+                  <c:v>1.04452939783475E-10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3948,7 +3958,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$23:$A$27</c:f>
+              <c:f>Sheet1!$A$33:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3972,24 +3982,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$23:$C$27</c:f>
+              <c:f>Sheet1!$C$33:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.3275327478062006E-5</c:v>
+                  <c:v>3.6133495493571098E-9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.3272685862591802E-5</c:v>
+                  <c:v>3.58601761314407E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.2933827343348602E-5</c:v>
+                  <c:v>9.8266068191216605E-10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2617904601325404E-5</c:v>
+                  <c:v>1.02034131630548E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.2518006423951497E-5</c:v>
+                  <c:v>1.15981075032377E-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4040,7 +4050,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$30:$A$34</c:f>
+              <c:f>Sheet1!$A$44:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4064,24 +4074,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$C$34</c:f>
+              <c:f>Sheet1!$C$44:$C$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.2465522705215594E-5</c:v>
+                  <c:v>7.2552432449926497E-14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.24643500220788E-5</c:v>
+                  <c:v>8.5630497752193801E-15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.2466296799958707E-5</c:v>
+                  <c:v>1.9967450179935801E-18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2468291488930903E-5</c:v>
+                  <c:v>2.23770026259195E-15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.2467334264881597E-5</c:v>
+                  <c:v>1.25480053373134E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4132,7 +4142,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$37:$A$41</c:f>
+              <c:f>Sheet1!$A$54:$A$58</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4156,24 +4166,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$37:$C$41</c:f>
+              <c:f>Sheet1!$C$54:$C$58</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.3614813035795307E-5</c:v>
+                  <c:v>7.2857381967918304E-9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.3614813035795307E-5</c:v>
+                  <c:v>7.2857381967918304E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.3455513367966293E-5</c:v>
+                  <c:v>4.1005294095570102E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2810567711688194E-5</c:v>
+                  <c:v>5.2462033741270401E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.2566615498012401E-5</c:v>
+                  <c:v>5.5698133673293799E-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4188,11 +4198,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="589243608"/>
-        <c:axId val="589242432"/>
+        <c:axId val="282795912"/>
+        <c:axId val="436759112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="589243608"/>
+        <c:axId val="282795912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10000"/>
@@ -4292,12 +4302,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="589242432"/>
+        <c:crossAx val="436759112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="589242432"/>
+        <c:axId val="436759112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4429,7 +4439,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="589243608"/>
+        <c:crossAx val="282795912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7126,10 +7136,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V41"/>
+  <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D23" zoomScale="96" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -7165,37 +7175,41 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
-        <v>7.2841918958479804E-7</v>
+        <v>1.4510244008709099E-6</v>
       </c>
       <c r="B2" s="1">
-        <v>2.8084443910738601E-4</v>
+        <v>2.1857214590375499E-8</v>
       </c>
       <c r="C2" s="1">
-        <v>4.7799977523737404E-7</v>
+        <v>7.0686529086884303E-7</v>
       </c>
       <c r="D2" s="1">
-        <v>2.8084443910738601E-4</v>
+        <v>2.1857214590375499E-8</v>
       </c>
       <c r="E2" s="1">
-        <v>1.6780930317487401E-7</v>
+        <v>1.5974736883292899E-7</v>
       </c>
       <c r="F2" s="1">
-        <v>2.8084443910738601E-4</v>
+        <v>2.1857214590375499E-8</v>
       </c>
       <c r="G2" s="1">
-        <v>2.2918945093584899E-8</v>
+        <v>2.3960736152945901E-8</v>
       </c>
       <c r="H2" s="1">
-        <v>2.7876878651046302E-4</v>
+        <v>3.0640327873730502E-9</v>
       </c>
       <c r="I2" s="1">
-        <v>4.8605569800906203E-9</v>
+        <v>3.8580355346083702E-9</v>
       </c>
       <c r="J2" s="1">
-        <v>2.77846248916882E-4</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+        <v>3.1520405020451002E-10</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1.9016566080095299E-9</v>
+      </c>
+      <c r="L2" s="1">
+        <v>3.1903593691417198E-11</v>
+      </c>
       <c r="O2" t="s">
         <v>12</v>
       </c>
@@ -7205,37 +7219,41 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
-        <v>2.8380796289791E-7</v>
+        <v>1.7932944029196901E-7</v>
       </c>
       <c r="B3" s="1">
-        <v>9.3614813035795307E-5</v>
+        <v>7.2857381967918304E-9</v>
       </c>
       <c r="C3" s="1">
-        <v>1.3675456029753599E-7</v>
+        <v>3.7246370449146702E-7</v>
       </c>
       <c r="D3" s="1">
-        <v>9.3614813035795307E-5</v>
+        <v>7.2857381967918304E-9</v>
       </c>
       <c r="E3" s="1">
-        <v>3.9183071390736901E-8</v>
+        <v>1.0453911621326E-7</v>
       </c>
       <c r="F3" s="1">
-        <v>9.3614813035795307E-5</v>
+        <v>7.2857381967918304E-9</v>
       </c>
       <c r="G3" s="1">
-        <v>1.1301042511442001E-8</v>
+        <v>1.27952673553787E-8</v>
       </c>
       <c r="H3" s="1">
-        <v>9.2913205979498306E-5</v>
+        <v>1.00899149306323E-9</v>
       </c>
       <c r="I3" s="1">
-        <v>1.50885690802169E-9</v>
+        <v>1.70838200365653E-9</v>
       </c>
       <c r="J3" s="1">
-        <v>9.2618474537597097E-5</v>
-      </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+        <v>1.04452939783475E-10</v>
+      </c>
+      <c r="K3" s="1">
+        <v>5.8434729134414604E-10</v>
+      </c>
+      <c r="L3" s="1">
+        <v>9.9248139202706294E-12</v>
+      </c>
       <c r="O3" t="s">
         <v>13</v>
       </c>
@@ -7245,37 +7263,41 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
-        <v>1.2226509928910699E-7</v>
+        <v>6.7026041219985505E-8</v>
       </c>
       <c r="B4" s="1">
-        <v>9.3275327478062006E-5</v>
+        <v>3.6133495493571098E-9</v>
       </c>
       <c r="C4" s="1">
-        <v>3.2018927582180697E-8</v>
+        <v>5.4946485086662899E-8</v>
       </c>
       <c r="D4" s="1">
-        <v>9.3272685862591802E-5</v>
+        <v>3.58601761314407E-9</v>
       </c>
       <c r="E4" s="1">
-        <v>2.1548136916757099E-8</v>
+        <v>9.9410512173473498E-9</v>
       </c>
       <c r="F4" s="1">
-        <v>9.2933827343348602E-5</v>
+        <v>9.8266068191216605E-10</v>
       </c>
       <c r="G4" s="1">
-        <v>1.6582931970523899E-9</v>
+        <v>1.97341778817197E-9</v>
       </c>
       <c r="H4" s="1">
-        <v>9.2617904601325404E-5</v>
+        <v>1.02034131630548E-10</v>
       </c>
       <c r="I4" s="1">
-        <v>4.6371932109278102E-10</v>
+        <v>4.8655405956019296E-10</v>
       </c>
       <c r="J4" s="1">
-        <v>9.2518006423951497E-5</v>
-      </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+        <v>1.15981075032377E-11</v>
+      </c>
+      <c r="K4" s="1">
+        <v>5.3388987196377097E-10</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1.1038044570242E-12</v>
+      </c>
       <c r="O4" t="s">
         <v>14</v>
       </c>
@@ -7285,37 +7307,41 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
-        <v>1.3131755228371001E-7</v>
+        <v>6.3325189237862194E-8</v>
       </c>
       <c r="B5" s="1">
-        <v>9.2465522705215594E-5</v>
+        <v>7.2552432449926497E-14</v>
       </c>
       <c r="C5" s="1">
-        <v>1.46869455247919E-7</v>
+        <v>1.16774127528446E-7</v>
       </c>
       <c r="D5" s="1">
-        <v>9.24643500220788E-5</v>
+        <v>8.5630497752193801E-15</v>
       </c>
       <c r="E5" s="1">
-        <v>3.1461888292308501E-8</v>
+        <v>4.4652915683968E-8</v>
       </c>
       <c r="F5" s="1">
-        <v>9.2466296799958707E-5</v>
+        <v>1.9967450179935801E-18</v>
       </c>
       <c r="G5" s="1">
-        <v>4.0066208912654796E-9</v>
+        <v>3.8425043965408002E-9</v>
       </c>
       <c r="H5" s="1">
-        <v>9.2468291488930903E-5</v>
+        <v>2.23770026259195E-15</v>
       </c>
       <c r="I5" s="1">
-        <v>9.9031282642286391E-10</v>
+        <v>1.1005629710667E-9</v>
       </c>
       <c r="J5" s="1">
-        <v>9.2467334264881597E-5</v>
-      </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+        <v>1.25480053373134E-15</v>
+      </c>
+      <c r="K5" s="1">
+        <v>5.6717556885108595E-10</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1.2795427653019601E-16</v>
+      </c>
       <c r="O5" t="s">
         <v>15</v>
       </c>
@@ -7325,37 +7351,41 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
-        <v>2.2329631936035599E-7</v>
+        <v>5.6771458938979796E-7</v>
       </c>
       <c r="B6" s="1">
-        <v>9.3614813035795307E-5</v>
+        <v>7.2857381967918304E-9</v>
       </c>
       <c r="C6" s="1">
-        <v>1.1163338770654499E-7</v>
+        <v>2.1569138208979601E-7</v>
       </c>
       <c r="D6" s="1">
-        <v>9.3614813035795307E-5</v>
+        <v>7.2857381967918304E-9</v>
       </c>
       <c r="E6" s="1">
-        <v>8.1843696559632905E-8</v>
+        <v>4.43760945555107E-8</v>
       </c>
       <c r="F6" s="1">
-        <v>9.3455513367966293E-5</v>
+        <v>4.1005294095570102E-9</v>
       </c>
       <c r="G6" s="1">
-        <v>4.77673000217923E-9</v>
+        <v>4.7120170133968798E-9</v>
       </c>
       <c r="H6" s="1">
-        <v>9.2810567711688194E-5</v>
+        <v>5.2462033741270401E-10</v>
       </c>
       <c r="I6" s="1">
-        <v>1.00435672696243E-9</v>
+        <v>8.1723315720573001E-10</v>
       </c>
       <c r="J6" s="1">
-        <v>9.2566615498012401E-5</v>
-      </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+        <v>5.5698133673293799E-11</v>
+      </c>
+      <c r="K6" s="1">
+        <v>6.5683891266335601E-10</v>
+      </c>
+      <c r="L6" s="1">
+        <v>5.7377231125036202E-12</v>
+      </c>
       <c r="O6" t="s">
         <v>16</v>
       </c>
@@ -7364,142 +7394,91 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
       <c r="V8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A9" s="1">
-        <v>24221</v>
-      </c>
-      <c r="B9" s="1">
-        <v>7.2841918958479804E-7</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2.8084443910738601E-4</v>
-      </c>
       <c r="V9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A10" s="1">
-        <v>48442</v>
-      </c>
-      <c r="B10" s="1">
-        <v>4.7799977523737404E-7</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2.8084443910738601E-4</v>
-      </c>
-    </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A11" s="1">
-        <v>242210</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1.6780930317487401E-7</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2.8084443910738601E-4</v>
-      </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A12" s="1">
-        <v>2422100</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2.2918945093584899E-8</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2.7876878651046302E-4</v>
-      </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A13" s="1">
-        <v>24221000</v>
-      </c>
-      <c r="B13" s="1">
-        <v>4.8605569800906203E-9</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2.77846248916882E-4</v>
+      <c r="B13" t="s">
+        <v>6</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
+      <c r="A14" s="1">
+        <v>24221</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.4510244008709099E-6</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2.1857214590375499E-8</v>
+      </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="B15" s="1" t="s">
-        <v>7</v>
+      <c r="A15" s="1">
+        <v>48442</v>
+      </c>
+      <c r="B15" s="1">
+        <v>7.0686529086884303E-7</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2.1857214590375499E-8</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
-        <v>24221</v>
+        <v>242210</v>
       </c>
       <c r="B16" s="1">
-        <v>2.8380796289791E-7</v>
+        <v>1.5974736883292899E-7</v>
       </c>
       <c r="C16" s="1">
-        <v>9.3614813035795307E-5</v>
+        <v>2.1857214590375499E-8</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
-        <v>48442</v>
+        <v>2422100</v>
       </c>
       <c r="B17" s="1">
-        <v>1.3675456029753599E-7</v>
+        <v>2.3960736152945901E-8</v>
       </c>
       <c r="C17" s="1">
-        <v>9.3614813035795307E-5</v>
+        <v>3.0640327873730502E-9</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
-        <v>242210</v>
+        <v>24221000</v>
       </c>
       <c r="B18" s="1">
-        <v>3.9183071390736901E-8</v>
+        <v>3.8580355346083702E-9</v>
       </c>
       <c r="C18" s="1">
-        <v>9.3614813035795307E-5</v>
+        <v>3.1520405020451002E-10</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19" s="1">
-        <v>2422100</v>
-      </c>
-      <c r="B19" s="1">
-        <v>1.1301042511442001E-8</v>
-      </c>
-      <c r="C19" s="1">
-        <v>9.2913205979498306E-5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A20" s="1">
-        <v>24221000</v>
-      </c>
-      <c r="B20" s="1">
-        <v>1.50885690802169E-9</v>
-      </c>
-      <c r="C20" s="1">
-        <v>9.2618474537597097E-5</v>
-      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B22" t="s">
-        <v>8</v>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
@@ -7507,10 +7486,10 @@
         <v>24221</v>
       </c>
       <c r="B23" s="1">
-        <v>1.2226509928910699E-7</v>
+        <v>1.7932944029196901E-7</v>
       </c>
       <c r="C23" s="1">
-        <v>9.3275327478062006E-5</v>
+        <v>7.2857381967918304E-9</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
@@ -7518,10 +7497,10 @@
         <v>48442</v>
       </c>
       <c r="B24" s="1">
-        <v>3.2018927582180697E-8</v>
+        <v>3.7246370449146702E-7</v>
       </c>
       <c r="C24" s="1">
-        <v>9.3272685862591802E-5</v>
+        <v>7.2857381967918304E-9</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
@@ -7529,10 +7508,10 @@
         <v>242210</v>
       </c>
       <c r="B25" s="1">
-        <v>2.1548136916757099E-8</v>
+        <v>1.0453911621326E-7</v>
       </c>
       <c r="C25" s="1">
-        <v>9.2933827343348602E-5</v>
+        <v>7.2857381967918304E-9</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
@@ -7540,10 +7519,10 @@
         <v>2422100</v>
       </c>
       <c r="B26" s="1">
-        <v>1.6582931970523899E-9</v>
+        <v>1.27952673553787E-8</v>
       </c>
       <c r="C26" s="1">
-        <v>9.2617904601325404E-5</v>
+        <v>1.00899149306323E-9</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
@@ -7551,130 +7530,210 @@
         <v>24221000</v>
       </c>
       <c r="B27" s="1">
-        <v>4.6371932109278102E-10</v>
+        <v>1.70838200365653E-9</v>
       </c>
       <c r="C27" s="1">
-        <v>9.2518006423951497E-5</v>
+        <v>1.04452939783475E-10</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A30" s="1">
-        <v>24221</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1.3131755228371001E-7</v>
-      </c>
-      <c r="C30" s="1">
-        <v>9.2465522705215594E-5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A31" s="1">
-        <v>48442</v>
-      </c>
-      <c r="B31" s="1">
-        <v>1.46869455247919E-7</v>
-      </c>
-      <c r="C31" s="1">
-        <v>9.24643500220788E-5</v>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>242210000</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A32" s="1">
-        <v>242210</v>
-      </c>
-      <c r="B32" s="1">
-        <v>3.1461888292308501E-8</v>
-      </c>
-      <c r="C32" s="1">
-        <v>9.2466296799958707E-5</v>
+      <c r="B32" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" s="1">
-        <v>2422100</v>
+        <v>24221</v>
       </c>
       <c r="B33" s="1">
-        <v>4.0066208912654796E-9</v>
+        <v>6.7026041219985505E-8</v>
       </c>
       <c r="C33" s="1">
-        <v>9.2468291488930903E-5</v>
+        <v>3.6133495493571098E-9</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" s="1">
-        <v>24221000</v>
+        <v>48442</v>
       </c>
       <c r="B34" s="1">
-        <v>9.9031282642286391E-10</v>
+        <v>5.4946485086662899E-8</v>
       </c>
       <c r="C34" s="1">
-        <v>9.2467334264881597E-5</v>
+        <v>3.58601761314407E-9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A35" s="1">
+        <v>242210</v>
+      </c>
+      <c r="B35" s="1">
+        <v>9.9410512173473498E-9</v>
+      </c>
+      <c r="C35" s="1">
+        <v>9.8266068191216605E-10</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B36" t="s">
-        <v>10</v>
+      <c r="A36" s="1">
+        <v>2422100</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1.97341778817197E-9</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1.02034131630548E-10</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" s="1">
-        <v>24221</v>
+        <v>24221000</v>
       </c>
       <c r="B37" s="1">
-        <v>2.2329631936035599E-7</v>
+        <v>4.8655405956019296E-10</v>
       </c>
       <c r="C37" s="1">
-        <v>9.3614813035795307E-5</v>
+        <v>1.15981075032377E-11</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A38" s="1">
+      <c r="A38">
+        <v>242210000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A44" s="1">
+        <v>24221</v>
+      </c>
+      <c r="B44" s="1">
+        <v>6.3325189237862194E-8</v>
+      </c>
+      <c r="C44" s="1">
+        <v>7.2552432449926497E-14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A45" s="1">
         <v>48442</v>
       </c>
-      <c r="B38" s="1">
-        <v>1.1163338770654499E-7</v>
-      </c>
-      <c r="C38" s="1">
-        <v>9.3614813035795307E-5</v>
+      <c r="B45" s="1">
+        <v>1.16774127528446E-7</v>
+      </c>
+      <c r="C45" s="1">
+        <v>8.5630497752193801E-15</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A39" s="1">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A46" s="1">
         <v>242210</v>
       </c>
-      <c r="B39" s="1">
-        <v>8.1843696559632905E-8</v>
-      </c>
-      <c r="C39" s="1">
-        <v>9.3455513367966293E-5</v>
+      <c r="B46" s="1">
+        <v>4.4652915683968E-8</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1.9967450179935801E-18</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A40" s="1">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A47" s="1">
         <v>2422100</v>
       </c>
-      <c r="B40" s="1">
-        <v>4.77673000217923E-9</v>
-      </c>
-      <c r="C40" s="1">
-        <v>9.2810567711688194E-5</v>
+      <c r="B47" s="1">
+        <v>3.8425043965408002E-9</v>
+      </c>
+      <c r="C47" s="1">
+        <v>2.23770026259195E-15</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A41" s="1">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A48" s="1">
         <v>24221000</v>
       </c>
-      <c r="B41" s="1">
-        <v>1.00435672696243E-9</v>
-      </c>
-      <c r="C41" s="1">
-        <v>9.2566615498012401E-5</v>
+      <c r="B48" s="1">
+        <v>1.1005629710667E-9</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1.25480053373134E-15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A49">
+        <v>242210000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A54" s="1">
+        <v>24221</v>
+      </c>
+      <c r="B54" s="1">
+        <v>5.6771458938979796E-7</v>
+      </c>
+      <c r="C54" s="1">
+        <v>7.2857381967918304E-9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A55" s="1">
+        <v>48442</v>
+      </c>
+      <c r="B55" s="1">
+        <v>2.1569138208979601E-7</v>
+      </c>
+      <c r="C55" s="1">
+        <v>7.2857381967918304E-9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A56" s="1">
+        <v>242210</v>
+      </c>
+      <c r="B56" s="1">
+        <v>4.43760945555107E-8</v>
+      </c>
+      <c r="C56" s="1">
+        <v>4.1005294095570102E-9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A57" s="1">
+        <v>2422100</v>
+      </c>
+      <c r="B57" s="1">
+        <v>4.7120170133968798E-9</v>
+      </c>
+      <c r="C57" s="1">
+        <v>5.2462033741270401E-10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A58" s="1">
+        <v>24221000</v>
+      </c>
+      <c r="B58" s="1">
+        <v>8.1723315720573001E-10</v>
+      </c>
+      <c r="C58" s="1">
+        <v>5.5698133673293799E-11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A59">
+        <v>242210000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>